<commit_message>
add additional check for duplicate veris path or duplicate mapping within the same veris path
</commit_message>
<xml_diff>
--- a/frameworks/veris/veris-mappings.xlsx
+++ b/frameworks/veris/veris-mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmanuelle\Documents\GitHub\attack_to_veris\frameworks\veris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2734D9D3-805F-4739-B31B-3417ECD9D1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125E9260-D7FE-4AC2-87C8-0C341FF77338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25485" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="8" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3937" uniqueCount="1421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3934" uniqueCount="1421">
   <si>
     <t>Use of stolen creds</t>
   </si>
@@ -5121,7 +5121,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62726C7-AE57-47B4-AC07-9EA1C9A6C528}">
   <dimension ref="D6:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5178,7 +5180,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B670464-1153-4AA6-978E-5B7FAB2C4B98}">
   <dimension ref="A1:C770"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView topLeftCell="A562" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C600" sqref="C600"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13378,9 +13382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7AF39-A8AE-1448-8EA3-B969364DCC63}">
   <dimension ref="A1:D339"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16772,11 +16774,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CCB954-7F07-6146-AFEF-8ED5165CE356}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17274,136 +17274,125 @@
     </row>
     <row r="54" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="42" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B54" s="44" t="s">
-        <v>149</v>
+        <v>259</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>150</v>
+        <v>260</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="42" t="s">
-        <v>27</v>
-      </c>
+      <c r="A55" s="42"/>
       <c r="B55" s="44" t="s">
+        <v>559</v>
+      </c>
+      <c r="C55" s="42" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="44" t="s">
         <v>259</v>
       </c>
-      <c r="C55" s="42" t="s">
+      <c r="C56" s="42" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="42"/>
-      <c r="B56" s="44" t="s">
+    <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="42"/>
+      <c r="B57" s="44" t="s">
         <v>559</v>
       </c>
-      <c r="C56" s="42" t="s">
+      <c r="C57" s="42" t="s">
         <v>1240</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="44" t="s">
-        <v>259</v>
-      </c>
-      <c r="C57" s="42" t="s">
-        <v>260</v>
-      </c>
-    </row>
     <row r="58" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="42"/>
+      <c r="A58" s="42" t="s">
+        <v>22</v>
+      </c>
       <c r="B58" s="44" t="s">
-        <v>559</v>
+        <v>249</v>
       </c>
       <c r="C58" s="42" t="s">
-        <v>1240</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="42" t="s">
-        <v>22</v>
-      </c>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="42"/>
       <c r="B59" s="44" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="C59" s="42" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="42"/>
-      <c r="B60" s="44" t="s">
-        <v>230</v>
-      </c>
-      <c r="C60" s="42" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="54" t="s">
+        <v>385</v>
+      </c>
+      <c r="C60" s="73" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="42"/>
       <c r="B61" s="54" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C61" s="73" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="42"/>
       <c r="B62" s="54" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C62" s="73" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="42"/>
-      <c r="B63" s="54" t="s">
-        <v>382</v>
+        <v>873</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="44" t="s">
+        <v>161</v>
       </c>
       <c r="C63" s="73" t="s">
-        <v>873</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B64" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C64" s="73" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B64" s="44"/>
+      <c r="C64" s="42"/>
+    </row>
+    <row r="65" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="42" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B65" s="44"/>
       <c r="C65" s="42"/>
     </row>
-    <row r="66" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" s="44"/>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="43" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B66" s="5"/>
       <c r="C66" s="42"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="43" t="s">
-        <v>1215</v>
-      </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="42"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="41" t="s">
+      <c r="A67" s="41" t="s">
         <v>1227</v>
       </c>
     </row>
@@ -17439,45 +17428,44 @@
     <hyperlink ref="B8" r:id="rId28" xr:uid="{86A41023-0140-4848-8EF6-50446073F042}"/>
     <hyperlink ref="B2" r:id="rId29" xr:uid="{33ABDE85-4705-4552-BFD2-3CFFB6F0FF7A}"/>
     <hyperlink ref="B41" r:id="rId30" display="T1059 " xr:uid="{68B8C08C-425A-42E0-B378-EEEE273ADC9B}"/>
-    <hyperlink ref="B60" r:id="rId31" xr:uid="{30499F46-B3B9-419B-9A95-798E4A458117}"/>
-    <hyperlink ref="B59" r:id="rId32" xr:uid="{A3B3CBA7-E2BF-40C1-B0D5-E1331591B1B2}"/>
-    <hyperlink ref="B58" r:id="rId33" xr:uid="{1985B65B-6872-4CA1-8126-B38AFAE9F259}"/>
-    <hyperlink ref="B57" r:id="rId34" xr:uid="{5E862F0C-0A49-4386-B708-CF885DCC7580}"/>
-    <hyperlink ref="B56" r:id="rId35" xr:uid="{3356D9BF-9EFB-4AB8-BB4C-5B42B5050D8D}"/>
-    <hyperlink ref="B55" r:id="rId36" xr:uid="{682BC205-7E4D-4C21-BB7F-28FC0BBC722E}"/>
-    <hyperlink ref="B54" r:id="rId37" xr:uid="{163EA14F-1883-4FC4-AF3A-C220BDAA547F}"/>
-    <hyperlink ref="B42:B46" r:id="rId38" display="T1059.001" xr:uid="{6ABC2D0F-A1AA-487F-9082-C8AC31BF0A05}"/>
-    <hyperlink ref="B47:B49" r:id="rId39" display="T1059.006" xr:uid="{96CA3176-C2E2-4FB3-AC05-163DBDD58192}"/>
-    <hyperlink ref="B42" r:id="rId40" xr:uid="{D07D00EE-9256-4C73-BB87-FB5E83FCAD24}"/>
-    <hyperlink ref="B43" r:id="rId41" xr:uid="{467D74DB-DA67-4F7C-84F8-3C580FE97C7C}"/>
-    <hyperlink ref="B44" r:id="rId42" xr:uid="{74F7E318-E403-446A-BEFE-0857CA7EEB15}"/>
-    <hyperlink ref="B45" r:id="rId43" xr:uid="{39E92F73-C43C-4593-B47A-900A7AC9084F}"/>
-    <hyperlink ref="B46" r:id="rId44" xr:uid="{3AB3A03D-BBA4-443D-B0BF-2C61DB5A365E}"/>
-    <hyperlink ref="B47" r:id="rId45" xr:uid="{F46ED575-9E55-4A15-9EA2-1B2C7C80A162}"/>
-    <hyperlink ref="B48" r:id="rId46" xr:uid="{3A4CA31A-96A8-4FD5-8A96-A95684E76E25}"/>
-    <hyperlink ref="B49" r:id="rId47" xr:uid="{372B438C-D56C-45B7-8A03-70AA0739A74A}"/>
-    <hyperlink ref="B64" r:id="rId48" xr:uid="{167C71DD-0469-4F2F-BBBD-31BAA6E67B40}"/>
-    <hyperlink ref="B52" r:id="rId49" xr:uid="{53E3529A-3621-443C-9B1B-A81282896161}"/>
-    <hyperlink ref="B61:B63" r:id="rId50" display="T1195.001" xr:uid="{B6AFA62A-D8E7-4B32-8175-5B2AF2804155}"/>
-    <hyperlink ref="B61" r:id="rId51" xr:uid="{CEA3D4B9-8C0E-4E93-AE50-2995881166FB}"/>
-    <hyperlink ref="B62" r:id="rId52" xr:uid="{A5B87B72-14F5-457E-932E-A66BCD902221}"/>
-    <hyperlink ref="B63" r:id="rId53" xr:uid="{4F93985E-E487-4B01-9F79-962F30C5511A}"/>
-    <hyperlink ref="B40" r:id="rId54" xr:uid="{EB78D91D-70C7-4478-868E-600B3110AD16}"/>
-    <hyperlink ref="B50" r:id="rId55" xr:uid="{D25BBB43-7188-47DD-B170-49DA47F39CC9}"/>
-    <hyperlink ref="B51" r:id="rId56" xr:uid="{14C90671-469E-4F32-8856-B7E75BE2C046}"/>
-    <hyperlink ref="B36" r:id="rId57" xr:uid="{D805DE71-F88D-4392-AF6D-0F1612C24BCA}"/>
-    <hyperlink ref="B37" r:id="rId58" xr:uid="{BBCD66C0-CDB0-41F5-B155-2FE87523FD6C}"/>
-    <hyperlink ref="B38" r:id="rId59" xr:uid="{2F54B841-CE28-4D19-BD70-BA02EC9C07BF}"/>
-    <hyperlink ref="B39" r:id="rId60" xr:uid="{2DF33F16-05A1-46AF-AF5C-2D258325E3BD}"/>
-    <hyperlink ref="B53" r:id="rId61" xr:uid="{34FC304F-2DFC-494F-B80E-1B479DD7939C}"/>
-    <hyperlink ref="B24" r:id="rId62" xr:uid="{E37FA0C1-118F-4E88-BEB8-BE70BD13A876}"/>
-    <hyperlink ref="B21" r:id="rId63" xr:uid="{CC7A808F-7C62-4A48-B407-A7D92A736DEB}"/>
-    <hyperlink ref="B22:B23" r:id="rId64" display="T1505.001" xr:uid="{DB01AC37-AC5E-4EEA-A504-F53DD1DB0949}"/>
-    <hyperlink ref="B22" r:id="rId65" xr:uid="{F1293C3B-8A5D-4869-B184-97F726B2A42D}"/>
-    <hyperlink ref="B23" r:id="rId66" xr:uid="{7ECCAE82-28DA-4075-AA3A-9F682393D745}"/>
+    <hyperlink ref="B59" r:id="rId31" xr:uid="{30499F46-B3B9-419B-9A95-798E4A458117}"/>
+    <hyperlink ref="B58" r:id="rId32" xr:uid="{A3B3CBA7-E2BF-40C1-B0D5-E1331591B1B2}"/>
+    <hyperlink ref="B57" r:id="rId33" xr:uid="{1985B65B-6872-4CA1-8126-B38AFAE9F259}"/>
+    <hyperlink ref="B56" r:id="rId34" xr:uid="{5E862F0C-0A49-4386-B708-CF885DCC7580}"/>
+    <hyperlink ref="B55" r:id="rId35" xr:uid="{3356D9BF-9EFB-4AB8-BB4C-5B42B5050D8D}"/>
+    <hyperlink ref="B54" r:id="rId36" xr:uid="{682BC205-7E4D-4C21-BB7F-28FC0BBC722E}"/>
+    <hyperlink ref="B42:B46" r:id="rId37" display="T1059.001" xr:uid="{6ABC2D0F-A1AA-487F-9082-C8AC31BF0A05}"/>
+    <hyperlink ref="B47:B49" r:id="rId38" display="T1059.006" xr:uid="{96CA3176-C2E2-4FB3-AC05-163DBDD58192}"/>
+    <hyperlink ref="B42" r:id="rId39" xr:uid="{D07D00EE-9256-4C73-BB87-FB5E83FCAD24}"/>
+    <hyperlink ref="B43" r:id="rId40" xr:uid="{467D74DB-DA67-4F7C-84F8-3C580FE97C7C}"/>
+    <hyperlink ref="B44" r:id="rId41" xr:uid="{74F7E318-E403-446A-BEFE-0857CA7EEB15}"/>
+    <hyperlink ref="B45" r:id="rId42" xr:uid="{39E92F73-C43C-4593-B47A-900A7AC9084F}"/>
+    <hyperlink ref="B46" r:id="rId43" xr:uid="{3AB3A03D-BBA4-443D-B0BF-2C61DB5A365E}"/>
+    <hyperlink ref="B47" r:id="rId44" xr:uid="{F46ED575-9E55-4A15-9EA2-1B2C7C80A162}"/>
+    <hyperlink ref="B48" r:id="rId45" xr:uid="{3A4CA31A-96A8-4FD5-8A96-A95684E76E25}"/>
+    <hyperlink ref="B49" r:id="rId46" xr:uid="{372B438C-D56C-45B7-8A03-70AA0739A74A}"/>
+    <hyperlink ref="B63" r:id="rId47" xr:uid="{167C71DD-0469-4F2F-BBBD-31BAA6E67B40}"/>
+    <hyperlink ref="B52" r:id="rId48" xr:uid="{53E3529A-3621-443C-9B1B-A81282896161}"/>
+    <hyperlink ref="B60:B62" r:id="rId49" display="T1195.001" xr:uid="{B6AFA62A-D8E7-4B32-8175-5B2AF2804155}"/>
+    <hyperlink ref="B60" r:id="rId50" xr:uid="{CEA3D4B9-8C0E-4E93-AE50-2995881166FB}"/>
+    <hyperlink ref="B61" r:id="rId51" xr:uid="{A5B87B72-14F5-457E-932E-A66BCD902221}"/>
+    <hyperlink ref="B62" r:id="rId52" xr:uid="{4F93985E-E487-4B01-9F79-962F30C5511A}"/>
+    <hyperlink ref="B40" r:id="rId53" xr:uid="{EB78D91D-70C7-4478-868E-600B3110AD16}"/>
+    <hyperlink ref="B50" r:id="rId54" xr:uid="{D25BBB43-7188-47DD-B170-49DA47F39CC9}"/>
+    <hyperlink ref="B51" r:id="rId55" xr:uid="{14C90671-469E-4F32-8856-B7E75BE2C046}"/>
+    <hyperlink ref="B36" r:id="rId56" xr:uid="{D805DE71-F88D-4392-AF6D-0F1612C24BCA}"/>
+    <hyperlink ref="B37" r:id="rId57" xr:uid="{BBCD66C0-CDB0-41F5-B155-2FE87523FD6C}"/>
+    <hyperlink ref="B38" r:id="rId58" xr:uid="{2F54B841-CE28-4D19-BD70-BA02EC9C07BF}"/>
+    <hyperlink ref="B39" r:id="rId59" xr:uid="{2DF33F16-05A1-46AF-AF5C-2D258325E3BD}"/>
+    <hyperlink ref="B53" r:id="rId60" xr:uid="{34FC304F-2DFC-494F-B80E-1B479DD7939C}"/>
+    <hyperlink ref="B24" r:id="rId61" xr:uid="{E37FA0C1-118F-4E88-BEB8-BE70BD13A876}"/>
+    <hyperlink ref="B21" r:id="rId62" xr:uid="{CC7A808F-7C62-4A48-B407-A7D92A736DEB}"/>
+    <hyperlink ref="B22:B23" r:id="rId63" display="T1505.001" xr:uid="{DB01AC37-AC5E-4EEA-A504-F53DD1DB0949}"/>
+    <hyperlink ref="B22" r:id="rId64" xr:uid="{F1293C3B-8A5D-4869-B184-97F726B2A42D}"/>
+    <hyperlink ref="B23" r:id="rId65" xr:uid="{7ECCAE82-28DA-4075-AA3A-9F682393D745}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId67"/>
+  <pageSetup orientation="portrait" r:id="rId66"/>
 </worksheet>
 </file>
 
@@ -17485,9 +17473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDB77F8-08D1-470F-BA2C-78FD3244C97D}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18227,9 +18213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFA46F8-B8B6-4B4E-AEB2-FE94B78BB5E8}">
   <dimension ref="A1:D310"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21390,9 +21374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F116B5EF-15D8-184F-A1F1-37879E79719C}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21809,9 +21791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EA7EB1-B9B4-4972-A1E8-8A90E68D0056}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22150,9 +22130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDF027E-A5AB-4362-BE7D-1C98B64C4E42}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22280,9 +22258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB4D0C4-AB00-444A-B726-674C8A391D6C}">
   <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Edits to validation script, documentation, and dependency (#28)
* add additional check for duplicate veris path or duplicate mapping within the same veris path

* move `stix2` dependency to latest 3.0.0

* couple of typo fixes or documentation
</commit_message>
<xml_diff>
--- a/frameworks/veris/veris-mappings.xlsx
+++ b/frameworks/veris/veris-mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmanuelle\Documents\GitHub\attack_to_veris\frameworks\veris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2734D9D3-805F-4739-B31B-3417ECD9D1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125E9260-D7FE-4AC2-87C8-0C341FF77338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25485" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="8" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3937" uniqueCount="1421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3934" uniqueCount="1421">
   <si>
     <t>Use of stolen creds</t>
   </si>
@@ -5121,7 +5121,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62726C7-AE57-47B4-AC07-9EA1C9A6C528}">
   <dimension ref="D6:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5178,7 +5180,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B670464-1153-4AA6-978E-5B7FAB2C4B98}">
   <dimension ref="A1:C770"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView topLeftCell="A562" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C600" sqref="C600"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13378,9 +13382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7AF39-A8AE-1448-8EA3-B969364DCC63}">
   <dimension ref="A1:D339"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16772,11 +16774,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CCB954-7F07-6146-AFEF-8ED5165CE356}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17274,136 +17274,125 @@
     </row>
     <row r="54" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="42" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B54" s="44" t="s">
-        <v>149</v>
+        <v>259</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>150</v>
+        <v>260</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="42" t="s">
-        <v>27</v>
-      </c>
+      <c r="A55" s="42"/>
       <c r="B55" s="44" t="s">
+        <v>559</v>
+      </c>
+      <c r="C55" s="42" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="44" t="s">
         <v>259</v>
       </c>
-      <c r="C55" s="42" t="s">
+      <c r="C56" s="42" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="42"/>
-      <c r="B56" s="44" t="s">
+    <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="42"/>
+      <c r="B57" s="44" t="s">
         <v>559</v>
       </c>
-      <c r="C56" s="42" t="s">
+      <c r="C57" s="42" t="s">
         <v>1240</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="44" t="s">
-        <v>259</v>
-      </c>
-      <c r="C57" s="42" t="s">
-        <v>260</v>
-      </c>
-    </row>
     <row r="58" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="42"/>
+      <c r="A58" s="42" t="s">
+        <v>22</v>
+      </c>
       <c r="B58" s="44" t="s">
-        <v>559</v>
+        <v>249</v>
       </c>
       <c r="C58" s="42" t="s">
-        <v>1240</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="42" t="s">
-        <v>22</v>
-      </c>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="42"/>
       <c r="B59" s="44" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="C59" s="42" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="42"/>
-      <c r="B60" s="44" t="s">
-        <v>230</v>
-      </c>
-      <c r="C60" s="42" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="54" t="s">
+        <v>385</v>
+      </c>
+      <c r="C60" s="73" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="42"/>
       <c r="B61" s="54" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C61" s="73" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="42"/>
       <c r="B62" s="54" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C62" s="73" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="42"/>
-      <c r="B63" s="54" t="s">
-        <v>382</v>
+        <v>873</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="44" t="s">
+        <v>161</v>
       </c>
       <c r="C63" s="73" t="s">
-        <v>873</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B64" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C64" s="73" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B64" s="44"/>
+      <c r="C64" s="42"/>
+    </row>
+    <row r="65" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="42" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B65" s="44"/>
       <c r="C65" s="42"/>
     </row>
-    <row r="66" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" s="44"/>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="43" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B66" s="5"/>
       <c r="C66" s="42"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="43" t="s">
-        <v>1215</v>
-      </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="42"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="41" t="s">
+      <c r="A67" s="41" t="s">
         <v>1227</v>
       </c>
     </row>
@@ -17439,45 +17428,44 @@
     <hyperlink ref="B8" r:id="rId28" xr:uid="{86A41023-0140-4848-8EF6-50446073F042}"/>
     <hyperlink ref="B2" r:id="rId29" xr:uid="{33ABDE85-4705-4552-BFD2-3CFFB6F0FF7A}"/>
     <hyperlink ref="B41" r:id="rId30" display="T1059 " xr:uid="{68B8C08C-425A-42E0-B378-EEEE273ADC9B}"/>
-    <hyperlink ref="B60" r:id="rId31" xr:uid="{30499F46-B3B9-419B-9A95-798E4A458117}"/>
-    <hyperlink ref="B59" r:id="rId32" xr:uid="{A3B3CBA7-E2BF-40C1-B0D5-E1331591B1B2}"/>
-    <hyperlink ref="B58" r:id="rId33" xr:uid="{1985B65B-6872-4CA1-8126-B38AFAE9F259}"/>
-    <hyperlink ref="B57" r:id="rId34" xr:uid="{5E862F0C-0A49-4386-B708-CF885DCC7580}"/>
-    <hyperlink ref="B56" r:id="rId35" xr:uid="{3356D9BF-9EFB-4AB8-BB4C-5B42B5050D8D}"/>
-    <hyperlink ref="B55" r:id="rId36" xr:uid="{682BC205-7E4D-4C21-BB7F-28FC0BBC722E}"/>
-    <hyperlink ref="B54" r:id="rId37" xr:uid="{163EA14F-1883-4FC4-AF3A-C220BDAA547F}"/>
-    <hyperlink ref="B42:B46" r:id="rId38" display="T1059.001" xr:uid="{6ABC2D0F-A1AA-487F-9082-C8AC31BF0A05}"/>
-    <hyperlink ref="B47:B49" r:id="rId39" display="T1059.006" xr:uid="{96CA3176-C2E2-4FB3-AC05-163DBDD58192}"/>
-    <hyperlink ref="B42" r:id="rId40" xr:uid="{D07D00EE-9256-4C73-BB87-FB5E83FCAD24}"/>
-    <hyperlink ref="B43" r:id="rId41" xr:uid="{467D74DB-DA67-4F7C-84F8-3C580FE97C7C}"/>
-    <hyperlink ref="B44" r:id="rId42" xr:uid="{74F7E318-E403-446A-BEFE-0857CA7EEB15}"/>
-    <hyperlink ref="B45" r:id="rId43" xr:uid="{39E92F73-C43C-4593-B47A-900A7AC9084F}"/>
-    <hyperlink ref="B46" r:id="rId44" xr:uid="{3AB3A03D-BBA4-443D-B0BF-2C61DB5A365E}"/>
-    <hyperlink ref="B47" r:id="rId45" xr:uid="{F46ED575-9E55-4A15-9EA2-1B2C7C80A162}"/>
-    <hyperlink ref="B48" r:id="rId46" xr:uid="{3A4CA31A-96A8-4FD5-8A96-A95684E76E25}"/>
-    <hyperlink ref="B49" r:id="rId47" xr:uid="{372B438C-D56C-45B7-8A03-70AA0739A74A}"/>
-    <hyperlink ref="B64" r:id="rId48" xr:uid="{167C71DD-0469-4F2F-BBBD-31BAA6E67B40}"/>
-    <hyperlink ref="B52" r:id="rId49" xr:uid="{53E3529A-3621-443C-9B1B-A81282896161}"/>
-    <hyperlink ref="B61:B63" r:id="rId50" display="T1195.001" xr:uid="{B6AFA62A-D8E7-4B32-8175-5B2AF2804155}"/>
-    <hyperlink ref="B61" r:id="rId51" xr:uid="{CEA3D4B9-8C0E-4E93-AE50-2995881166FB}"/>
-    <hyperlink ref="B62" r:id="rId52" xr:uid="{A5B87B72-14F5-457E-932E-A66BCD902221}"/>
-    <hyperlink ref="B63" r:id="rId53" xr:uid="{4F93985E-E487-4B01-9F79-962F30C5511A}"/>
-    <hyperlink ref="B40" r:id="rId54" xr:uid="{EB78D91D-70C7-4478-868E-600B3110AD16}"/>
-    <hyperlink ref="B50" r:id="rId55" xr:uid="{D25BBB43-7188-47DD-B170-49DA47F39CC9}"/>
-    <hyperlink ref="B51" r:id="rId56" xr:uid="{14C90671-469E-4F32-8856-B7E75BE2C046}"/>
-    <hyperlink ref="B36" r:id="rId57" xr:uid="{D805DE71-F88D-4392-AF6D-0F1612C24BCA}"/>
-    <hyperlink ref="B37" r:id="rId58" xr:uid="{BBCD66C0-CDB0-41F5-B155-2FE87523FD6C}"/>
-    <hyperlink ref="B38" r:id="rId59" xr:uid="{2F54B841-CE28-4D19-BD70-BA02EC9C07BF}"/>
-    <hyperlink ref="B39" r:id="rId60" xr:uid="{2DF33F16-05A1-46AF-AF5C-2D258325E3BD}"/>
-    <hyperlink ref="B53" r:id="rId61" xr:uid="{34FC304F-2DFC-494F-B80E-1B479DD7939C}"/>
-    <hyperlink ref="B24" r:id="rId62" xr:uid="{E37FA0C1-118F-4E88-BEB8-BE70BD13A876}"/>
-    <hyperlink ref="B21" r:id="rId63" xr:uid="{CC7A808F-7C62-4A48-B407-A7D92A736DEB}"/>
-    <hyperlink ref="B22:B23" r:id="rId64" display="T1505.001" xr:uid="{DB01AC37-AC5E-4EEA-A504-F53DD1DB0949}"/>
-    <hyperlink ref="B22" r:id="rId65" xr:uid="{F1293C3B-8A5D-4869-B184-97F726B2A42D}"/>
-    <hyperlink ref="B23" r:id="rId66" xr:uid="{7ECCAE82-28DA-4075-AA3A-9F682393D745}"/>
+    <hyperlink ref="B59" r:id="rId31" xr:uid="{30499F46-B3B9-419B-9A95-798E4A458117}"/>
+    <hyperlink ref="B58" r:id="rId32" xr:uid="{A3B3CBA7-E2BF-40C1-B0D5-E1331591B1B2}"/>
+    <hyperlink ref="B57" r:id="rId33" xr:uid="{1985B65B-6872-4CA1-8126-B38AFAE9F259}"/>
+    <hyperlink ref="B56" r:id="rId34" xr:uid="{5E862F0C-0A49-4386-B708-CF885DCC7580}"/>
+    <hyperlink ref="B55" r:id="rId35" xr:uid="{3356D9BF-9EFB-4AB8-BB4C-5B42B5050D8D}"/>
+    <hyperlink ref="B54" r:id="rId36" xr:uid="{682BC205-7E4D-4C21-BB7F-28FC0BBC722E}"/>
+    <hyperlink ref="B42:B46" r:id="rId37" display="T1059.001" xr:uid="{6ABC2D0F-A1AA-487F-9082-C8AC31BF0A05}"/>
+    <hyperlink ref="B47:B49" r:id="rId38" display="T1059.006" xr:uid="{96CA3176-C2E2-4FB3-AC05-163DBDD58192}"/>
+    <hyperlink ref="B42" r:id="rId39" xr:uid="{D07D00EE-9256-4C73-BB87-FB5E83FCAD24}"/>
+    <hyperlink ref="B43" r:id="rId40" xr:uid="{467D74DB-DA67-4F7C-84F8-3C580FE97C7C}"/>
+    <hyperlink ref="B44" r:id="rId41" xr:uid="{74F7E318-E403-446A-BEFE-0857CA7EEB15}"/>
+    <hyperlink ref="B45" r:id="rId42" xr:uid="{39E92F73-C43C-4593-B47A-900A7AC9084F}"/>
+    <hyperlink ref="B46" r:id="rId43" xr:uid="{3AB3A03D-BBA4-443D-B0BF-2C61DB5A365E}"/>
+    <hyperlink ref="B47" r:id="rId44" xr:uid="{F46ED575-9E55-4A15-9EA2-1B2C7C80A162}"/>
+    <hyperlink ref="B48" r:id="rId45" xr:uid="{3A4CA31A-96A8-4FD5-8A96-A95684E76E25}"/>
+    <hyperlink ref="B49" r:id="rId46" xr:uid="{372B438C-D56C-45B7-8A03-70AA0739A74A}"/>
+    <hyperlink ref="B63" r:id="rId47" xr:uid="{167C71DD-0469-4F2F-BBBD-31BAA6E67B40}"/>
+    <hyperlink ref="B52" r:id="rId48" xr:uid="{53E3529A-3621-443C-9B1B-A81282896161}"/>
+    <hyperlink ref="B60:B62" r:id="rId49" display="T1195.001" xr:uid="{B6AFA62A-D8E7-4B32-8175-5B2AF2804155}"/>
+    <hyperlink ref="B60" r:id="rId50" xr:uid="{CEA3D4B9-8C0E-4E93-AE50-2995881166FB}"/>
+    <hyperlink ref="B61" r:id="rId51" xr:uid="{A5B87B72-14F5-457E-932E-A66BCD902221}"/>
+    <hyperlink ref="B62" r:id="rId52" xr:uid="{4F93985E-E487-4B01-9F79-962F30C5511A}"/>
+    <hyperlink ref="B40" r:id="rId53" xr:uid="{EB78D91D-70C7-4478-868E-600B3110AD16}"/>
+    <hyperlink ref="B50" r:id="rId54" xr:uid="{D25BBB43-7188-47DD-B170-49DA47F39CC9}"/>
+    <hyperlink ref="B51" r:id="rId55" xr:uid="{14C90671-469E-4F32-8856-B7E75BE2C046}"/>
+    <hyperlink ref="B36" r:id="rId56" xr:uid="{D805DE71-F88D-4392-AF6D-0F1612C24BCA}"/>
+    <hyperlink ref="B37" r:id="rId57" xr:uid="{BBCD66C0-CDB0-41F5-B155-2FE87523FD6C}"/>
+    <hyperlink ref="B38" r:id="rId58" xr:uid="{2F54B841-CE28-4D19-BD70-BA02EC9C07BF}"/>
+    <hyperlink ref="B39" r:id="rId59" xr:uid="{2DF33F16-05A1-46AF-AF5C-2D258325E3BD}"/>
+    <hyperlink ref="B53" r:id="rId60" xr:uid="{34FC304F-2DFC-494F-B80E-1B479DD7939C}"/>
+    <hyperlink ref="B24" r:id="rId61" xr:uid="{E37FA0C1-118F-4E88-BEB8-BE70BD13A876}"/>
+    <hyperlink ref="B21" r:id="rId62" xr:uid="{CC7A808F-7C62-4A48-B407-A7D92A736DEB}"/>
+    <hyperlink ref="B22:B23" r:id="rId63" display="T1505.001" xr:uid="{DB01AC37-AC5E-4EEA-A504-F53DD1DB0949}"/>
+    <hyperlink ref="B22" r:id="rId64" xr:uid="{F1293C3B-8A5D-4869-B184-97F726B2A42D}"/>
+    <hyperlink ref="B23" r:id="rId65" xr:uid="{7ECCAE82-28DA-4075-AA3A-9F682393D745}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId67"/>
+  <pageSetup orientation="portrait" r:id="rId66"/>
 </worksheet>
 </file>
 
@@ -17485,9 +17473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDB77F8-08D1-470F-BA2C-78FD3244C97D}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18227,9 +18213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFA46F8-B8B6-4B4E-AEB2-FE94B78BB5E8}">
   <dimension ref="A1:D310"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21390,9 +21374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F116B5EF-15D8-184F-A1F1-37879E79719C}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21809,9 +21791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EA7EB1-B9B4-4972-A1E8-8A90E68D0056}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22150,9 +22130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDF027E-A5AB-4362-BE7D-1C98B64C4E42}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22280,9 +22258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB4D0C4-AB00-444A-B726-674C8A391D6C}">
   <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>